<commit_message>
rerun for apr 2024
</commit_message>
<xml_diff>
--- a/output/Low Util Trainer - 2024-04.xlsx
+++ b/output/Low Util Trainer - 2024-04.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="144">
   <si>
     <t>class_date</t>
   </si>
@@ -109,7 +109,7 @@
     <t>12, 13, 15, 16, 18, 19</t>
   </si>
   <si>
-    <t>12, 13, 18, 19, 20</t>
+    <t>12, 13, 16, 18, 19, 20</t>
   </si>
   <si>
     <t>13, 15, 16, 17, 19</t>
@@ -136,9 +136,6 @@
     <t>13, 14, 17, 18, 19, 15</t>
   </si>
   <si>
-    <t>12, 13, 16, 18, 19, 20</t>
-  </si>
-  <si>
     <t>01 Apr</t>
   </si>
   <si>
@@ -187,168 +184,147 @@
     <t>12, 15, 16, 18, 19, 20</t>
   </si>
   <si>
-    <t>12, 14, 16, 19</t>
+    <t>12, 14, 16, 17, 19</t>
   </si>
   <si>
     <t>12, 14, 15, 17, 18, 19</t>
   </si>
   <si>
-    <t>16, 18, 19, 20</t>
-  </si>
-  <si>
     <t>09 Apr</t>
   </si>
   <si>
     <t>25 Apr</t>
   </si>
   <si>
+    <t>13, 14, 16, 17, 19, 20</t>
+  </si>
+  <si>
+    <t>13, 14, 15, 17, 18, 19</t>
+  </si>
+  <si>
+    <t>13, 14, 15, 17, 19, 18</t>
+  </si>
+  <si>
+    <t>14, 16, 18, 19, 20, 12</t>
+  </si>
+  <si>
+    <t>13, 15, 16, 17, 19, 20</t>
+  </si>
+  <si>
+    <t>12, 13, 14, 16, 18, 19</t>
+  </si>
+  <si>
+    <t>15, 16, 17, 19, 12</t>
+  </si>
+  <si>
+    <t>14, 17, 13, 16, 19, 20</t>
+  </si>
+  <si>
+    <t>12, 15, 16, 19, 20, 17</t>
+  </si>
+  <si>
+    <t>13, 14, 17, 15, 18, 19</t>
+  </si>
+  <si>
+    <t>13, 14, 15, 17, 18</t>
+  </si>
+  <si>
+    <t>12, 15, 16, 18, 19</t>
+  </si>
+  <si>
+    <t>13, 14, 16, 18, 19</t>
+  </si>
+  <si>
+    <t>12, 13, 15, 18, 19</t>
+  </si>
+  <si>
+    <t>12, 13, 16, 17, 19, 15</t>
+  </si>
+  <si>
+    <t>14, 15, 17, 13, 19</t>
+  </si>
+  <si>
+    <t>12, 14, 18, 19, 15, 17</t>
+  </si>
+  <si>
+    <t>14, 15, 16, 18, 19</t>
+  </si>
+  <si>
+    <t>12, 14, 16, 18, 19, 20</t>
+  </si>
+  <si>
+    <t>12, 13, 15, 17, 18, 19</t>
+  </si>
+  <si>
     <t>13, 14, 16, 17, 19</t>
   </si>
   <si>
-    <t>13, 14, 16, 17, 19, 20</t>
-  </si>
-  <si>
-    <t>13, 14, 15, 17, 18, 19</t>
-  </si>
-  <si>
-    <t>13, 14, 15, 17, 19, 18</t>
-  </si>
-  <si>
-    <t>14, 16, 18, 19, 20, 12</t>
-  </si>
-  <si>
-    <t>13, 15, 16, 17, 19, 20</t>
-  </si>
-  <si>
-    <t>12, 13, 14, 16, 18, 19</t>
-  </si>
-  <si>
-    <t>15, 16, 17, 19, 12</t>
-  </si>
-  <si>
-    <t>13, 15, 16, 18, 19</t>
-  </si>
-  <si>
-    <t>14, 17, 13, 16, 19, 20</t>
-  </si>
-  <si>
-    <t>12, 15, 16, 19, 20</t>
-  </si>
-  <si>
-    <t>13, 14, 17, 15, 18, 19</t>
-  </si>
-  <si>
-    <t>14, 15, 17, 18</t>
-  </si>
-  <si>
-    <t>12, 15, 16, 18, 19</t>
-  </si>
-  <si>
-    <t>13, 14, 16, 18, 19</t>
-  </si>
-  <si>
-    <t>12, 13, 15, 18, 19</t>
-  </si>
-  <si>
-    <t>12, 13, 16, 17, 19, 15</t>
+    <t>08 Apr</t>
+  </si>
+  <si>
+    <t>13, 14, 15, 17, 19, 20</t>
+  </si>
+  <si>
+    <t>12, 13, 15, 16, 19, 20</t>
+  </si>
+  <si>
+    <t>12, 13, 14, 17, 19, 20</t>
+  </si>
+  <si>
+    <t>12, 13, 14, 16, 18, 20</t>
+  </si>
+  <si>
+    <t>14, 16, 17, 18, 20</t>
+  </si>
+  <si>
+    <t>15, 16, 17, 19, 20</t>
+  </si>
+  <si>
+    <t>14, 19, 20, 16</t>
+  </si>
+  <si>
+    <t>13, 12, 19, 17</t>
+  </si>
+  <si>
+    <t>11, 13, 15, 16</t>
+  </si>
+  <si>
+    <t>12, 14, 15, 19, 20</t>
+  </si>
+  <si>
+    <t>14, 15, 18, 20, 16</t>
+  </si>
+  <si>
+    <t>14, 15, 18, 19</t>
+  </si>
+  <si>
+    <t>15, 16, 19, 20, 17</t>
+  </si>
+  <si>
+    <t>15, 16, 18, 19</t>
+  </si>
+  <si>
+    <t>19, 20, 15, 18</t>
+  </si>
+  <si>
+    <t>13, 17, 18, 14</t>
+  </si>
+  <si>
+    <t>13, 15, 19, 20, 17</t>
+  </si>
+  <si>
+    <t>14, 15, 19, 17</t>
+  </si>
+  <si>
+    <t>14, 16, 17, 19, 20</t>
+  </si>
+  <si>
+    <t>13, 15, 19</t>
   </si>
   <si>
     <t>15, 16, 17, 19</t>
   </si>
   <si>
-    <t>14, 15, 17, 13, 19</t>
-  </si>
-  <si>
-    <t>12, 14, 18, 19, 15, 17</t>
-  </si>
-  <si>
-    <t>14, 15, 16, 18, 19</t>
-  </si>
-  <si>
-    <t>12, 14, 16, 18, 19, 20</t>
-  </si>
-  <si>
-    <t>12, 13, 15, 17, 18, 19</t>
-  </si>
-  <si>
-    <t>14, 16, 17, 19</t>
-  </si>
-  <si>
-    <t>14, 15, 18, 19</t>
-  </si>
-  <si>
-    <t>08 Apr</t>
-  </si>
-  <si>
-    <t>13, 14, 15, 17, 19, 20</t>
-  </si>
-  <si>
-    <t>13, 16, 17, 19, 20</t>
-  </si>
-  <si>
-    <t>12, 13, 15, 16, 19, 20</t>
-  </si>
-  <si>
-    <t>12, 13, 14, 17, 19, 20</t>
-  </si>
-  <si>
-    <t>12, 13, 14, 16, 18, 20</t>
-  </si>
-  <si>
-    <t>14, 16, 17, 18, 20</t>
-  </si>
-  <si>
-    <t>15, 16, 17, 19, 20</t>
-  </si>
-  <si>
-    <t>14, 19, 20, 16</t>
-  </si>
-  <si>
-    <t>13, 12, 19, 17</t>
-  </si>
-  <si>
-    <t>11, 13, 15, 16</t>
-  </si>
-  <si>
-    <t>12, 14, 15, 19</t>
-  </si>
-  <si>
-    <t>14, 15, 18, 20, 16</t>
-  </si>
-  <si>
-    <t>15, 16, 19, 20, 17</t>
-  </si>
-  <si>
-    <t>15, 16, 18, 19</t>
-  </si>
-  <si>
-    <t>19, 20, 15, 18</t>
-  </si>
-  <si>
-    <t>13, 17, 18, 14</t>
-  </si>
-  <si>
-    <t>13, 15, 19, 20, 17</t>
-  </si>
-  <si>
-    <t>14, 15, 19, 17</t>
-  </si>
-  <si>
-    <t>13, 14, 15, 17, 18</t>
-  </si>
-  <si>
-    <t>14, 16, 17, 19, 20</t>
-  </si>
-  <si>
-    <t>15, 16, 19</t>
-  </si>
-  <si>
-    <t>13, 15, 19</t>
-  </si>
-  <si>
-    <t>15, 17, 19</t>
-  </si>
-  <si>
     <t>17, 19, 20, 15</t>
   </si>
   <si>
@@ -382,7 +358,7 @@
     <t>15, 16, 17, 19, 20, 12</t>
   </si>
   <si>
-    <t>12, 16, 17, 13</t>
+    <t>12, 16, 17, 19, 13</t>
   </si>
   <si>
     <t>12, 14, 15, 17, 18, 20</t>
@@ -397,10 +373,7 @@
     <t>13, 16, 18, 19, 20</t>
   </si>
   <si>
-    <t>14, 15, 18, 17</t>
-  </si>
-  <si>
-    <t>12, 16, 18, 19, 20</t>
+    <t>14, 15, 18, 19, 17</t>
   </si>
   <si>
     <t>13, 15, 16, 20, 18, 19</t>
@@ -424,30 +397,24 @@
     <t>17</t>
   </si>
   <si>
-    <t>12, 13, 19, 20</t>
-  </si>
-  <si>
-    <t>12, 13, 16, 17, 20</t>
+    <t>12, 13, 16, 19, 20</t>
+  </si>
+  <si>
+    <t>12, 13, 16, 17, 20, 19</t>
   </si>
   <si>
     <t>12, 14, 15, 20, 19, 16</t>
   </si>
   <si>
-    <t>15, 16</t>
-  </si>
-  <si>
-    <t>12, 13, 14, 16, 17</t>
-  </si>
-  <si>
-    <t>16, 17, 19, 20</t>
+    <t>13, 15, 17, 16</t>
+  </si>
+  <si>
+    <t>12, 13, 14, 16, 17, 20</t>
   </si>
   <si>
     <t>13, 14, 16, 19, 17</t>
   </si>
   <si>
-    <t>13, 15, 16, 19, 20, 18</t>
-  </si>
-  <si>
     <t>13, 15, 16, 20, 18</t>
   </si>
   <si>
@@ -463,7 +430,7 @@
     <t>12, 16, 18</t>
   </si>
   <si>
-    <t>13, 14, 18, 16</t>
+    <t>13, 14, 18, 19, 20, 16</t>
   </si>
   <si>
     <t>20</t>
@@ -475,28 +442,22 @@
     <t>15, 16, 17, 19, 12, 20</t>
   </si>
   <si>
-    <t>16, 19, 20, 15</t>
-  </si>
-  <si>
-    <t>20, 16, 19</t>
-  </si>
-  <si>
-    <t>12, 20, 16, 17, 18</t>
+    <t>12, 16, 17, 19, 20, 15</t>
+  </si>
+  <si>
+    <t>12, 15, 20, 16, 19</t>
+  </si>
+  <si>
+    <t>12, 13, 20, 16, 17, 18</t>
   </si>
   <si>
     <t>12, 15, 16, 17</t>
   </si>
   <si>
-    <t>14, 15, 16</t>
-  </si>
-  <si>
     <t>13, 15, 16, 17, 20, 19</t>
   </si>
   <si>
-    <t>13, 15, 17, 18, 20</t>
-  </si>
-  <si>
-    <t>16, 19, 17</t>
+    <t>13, 14, 15, 17, 18, 20</t>
   </si>
 </sst>
 </file>
@@ -980,7 +941,7 @@
         <v>27</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1103,7 +1064,7 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -1138,10 +1099,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D2">
         <v>6</v>
@@ -1155,7 +1116,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -1169,7 +1130,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -1183,7 +1144,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -1194,13 +1155,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1208,10 +1169,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -1222,10 +1183,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
         <v>56</v>
-      </c>
-      <c r="C8" t="s">
-        <v>59</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1236,10 +1197,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -1250,10 +1211,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -1267,7 +1228,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -1278,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -1292,10 +1253,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D13">
         <v>6</v>
@@ -1323,7 +1284,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -1334,13 +1295,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1348,10 +1309,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D17">
         <v>6</v>
@@ -1365,10 +1326,10 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>124</v>
+        <v>27</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1400,10 +1361,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D2">
         <v>6</v>
@@ -1417,7 +1378,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -1431,7 +1392,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -1445,7 +1406,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -1459,7 +1420,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -1470,10 +1431,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -1484,10 +1445,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1501,7 +1462,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -1512,7 +1473,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -1529,7 +1490,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -1543,7 +1504,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -1554,10 +1515,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D13">
         <v>6</v>
@@ -1585,7 +1546,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1596,10 +1557,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -1610,10 +1571,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D17">
         <v>6</v>
@@ -1627,7 +1588,7 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -1640,7 +1601,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1665,7 +1626,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1679,10 +1640,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1693,10 +1654,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1707,7 +1668,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -1721,10 +1682,10 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1735,10 +1696,10 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1746,13 +1707,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
         <v>56</v>
       </c>
-      <c r="C8" t="s">
-        <v>85</v>
-      </c>
       <c r="D8">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1763,10 +1724,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>137</v>
+        <v>60</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1777,7 +1738,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -1788,10 +1749,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -1802,13 +1763,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1816,13 +1777,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1830,10 +1791,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>142</v>
+        <v>50</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -1844,13 +1805,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="D15">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1858,13 +1819,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1872,27 +1833,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D18">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1927,7 +1874,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1941,7 +1888,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -1955,7 +1902,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -1969,10 +1916,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1983,7 +1930,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1994,13 +1941,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2008,13 +1955,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2025,10 +1972,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2039,10 +1986,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2053,7 +2000,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -2081,10 +2028,10 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>153</v>
+        <v>73</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2095,7 +2042,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -2109,10 +2056,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2123,10 +2070,10 @@
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2182,10 +2129,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2">
         <v>6</v>
@@ -2199,7 +2146,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -2213,7 +2160,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -2227,7 +2174,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -2238,10 +2185,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -2252,10 +2199,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -2266,10 +2213,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -2283,7 +2230,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -2308,10 +2255,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -2322,10 +2269,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -2339,10 +2286,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2353,7 +2300,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -2364,10 +2311,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15">
         <v>6</v>
@@ -2378,10 +2325,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
         <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
       </c>
       <c r="D16">
         <v>6</v>
@@ -2395,10 +2342,10 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2433,7 +2380,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2">
         <v>6</v>
@@ -2447,10 +2394,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2475,7 +2422,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -2489,7 +2436,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -2500,10 +2447,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
         <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>59</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -2531,7 +2478,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -2545,7 +2492,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -2573,7 +2520,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -2587,7 +2534,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D13">
         <v>6</v>
@@ -2601,7 +2548,7 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -2615,7 +2562,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D15">
         <v>6</v>
@@ -2626,10 +2573,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D16">
         <v>6</v>
@@ -2643,10 +2590,10 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2657,7 +2604,7 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -2671,7 +2618,7 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D19">
         <v>6</v>
@@ -2709,7 +2656,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D2">
         <v>6</v>
@@ -2723,7 +2670,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -2776,13 +2723,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2793,7 +2740,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -2807,7 +2754,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -2821,10 +2768,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2849,7 +2796,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -2863,7 +2810,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D13">
         <v>6</v>
@@ -2877,7 +2824,7 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -2891,7 +2838,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D15">
         <v>6</v>
@@ -2905,7 +2852,7 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D16">
         <v>6</v>
@@ -2919,7 +2866,7 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D17">
         <v>6</v>
@@ -2933,7 +2880,7 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -2968,13 +2915,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2985,7 +2932,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -2996,10 +2943,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -3010,7 +2957,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -3027,7 +2974,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -3041,7 +2988,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -3055,7 +3002,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -3066,10 +3013,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -3080,13 +3027,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3097,7 +3044,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -3111,10 +3058,10 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3122,10 +3069,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13">
         <v>6</v>
@@ -3136,10 +3083,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -3191,7 +3138,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D2">
         <v>6</v>
@@ -3205,10 +3152,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3216,10 +3163,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -3230,10 +3177,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -3244,10 +3191,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -3275,7 +3222,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -3317,7 +3264,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -3331,7 +3278,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -3342,7 +3289,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
@@ -3373,7 +3320,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15">
         <v>6</v>
@@ -3398,7 +3345,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
         <v>30</v>
@@ -3415,10 +3362,10 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3450,10 +3397,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -3467,7 +3414,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -3481,7 +3428,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -3495,7 +3442,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -3506,10 +3453,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -3520,13 +3467,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3534,10 +3481,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -3551,7 +3498,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -3565,7 +3512,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -3579,7 +3526,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -3593,7 +3540,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -3604,10 +3551,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -3618,10 +3565,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -3635,7 +3582,7 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -3649,7 +3596,7 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D16">
         <v>5</v>
@@ -3660,10 +3607,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -3674,10 +3621,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D18">
         <v>5</v>
@@ -3691,10 +3638,10 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3729,7 +3676,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -3743,10 +3690,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3757,7 +3704,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -3771,7 +3718,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -3785,7 +3732,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -3799,7 +3746,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -3813,7 +3760,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -3827,7 +3774,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -3841,7 +3788,7 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -3855,7 +3802,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -3869,7 +3816,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -3880,10 +3827,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D13">
         <v>6</v>
@@ -3897,7 +3844,7 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -3911,7 +3858,7 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D15">
         <v>5</v>

</xml_diff>